<commit_message>
IG update: added communication reason codes valueset
</commit_message>
<xml_diff>
--- a/v0.9/StructureDefinition-Communication.xlsx
+++ b/v0.9/StructureDefinition-Communication.xlsx
@@ -823,7 +823,7 @@
     <t>Codes for describing reasons for the occurrence of a communication.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/clinical-findings</t>
+    <t>https://ig.hcxprotocol.io/v0.9/ValueSet-communication-reason-codes.html</t>
   </si>
   <si>
     <t>Event.reasonCode</t>
@@ -1267,7 +1267,7 @@
     <col min="23" max="23" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.9609375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="73.0859375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="57.484375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="69.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="20.84375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="18.84765625" customWidth="true" bestFit="true"/>

</xml_diff>